<commit_message>
Fixes to memroy table were added.
</commit_message>
<xml_diff>
--- a/memory_table.xlsx
+++ b/memory_table.xlsx
@@ -389,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -436,6 +436,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,7 +725,7 @@
   <dimension ref="A2:O24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="25.5" x14ac:dyDescent="0.35"/>
@@ -752,7 +753,7 @@
       <c r="L2" s="27"/>
       <c r="M2" s="27"/>
       <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
+      <c r="O2" s="28"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
@@ -1483,7 +1484,7 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="A2:O2"/>
+    <mergeCell ref="A2:N2"/>
     <mergeCell ref="B23:N23"/>
     <mergeCell ref="N16:N17"/>
     <mergeCell ref="B5:N5"/>
@@ -1496,6 +1497,6 @@
     <mergeCell ref="N13:N14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>